<commit_message>
add version 3.0.0 & 3.1.0 pdfs
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcg3304\Desktop\kwittup_ui_mockup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878B174B-FF60-4E6D-A22A-7DFDAFB29396}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFE26AE-F841-44F4-A925-83ACD6649DFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120" activeTab="1" xr2:uid="{885A90D6-9FE9-4F46-9DB7-99CFD7526296}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="127">
   <si>
     <t>#</t>
   </si>
@@ -1366,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEF2C79-7016-406E-AC36-4999B2C298F8}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1401,6 +1401,9 @@
       <c r="B3" t="s">
         <v>61</v>
       </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1418,7 +1421,7 @@
         <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1428,6 +1431,9 @@
       <c r="B6" t="s">
         <v>65</v>
       </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1454,7 +1460,7 @@
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C10" t="s">
@@ -1476,8 +1482,11 @@
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,6 +1496,9 @@
       <c r="B13" t="s">
         <v>70</v>
       </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1507,7 +1519,7 @@
         <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1517,17 +1529,23 @@
       <c r="B16" t="s">
         <v>72</v>
       </c>
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>120</v>
       </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1538,6 +1556,9 @@
       <c r="B19" t="s">
         <v>74</v>
       </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1547,7 +1568,7 @@
         <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1605,6 +1626,9 @@
       <c r="B27" t="s">
         <v>82</v>
       </c>
+      <c r="C27" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1614,7 +1638,7 @@
         <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1651,16 +1675,22 @@
       <c r="B32" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>29</v>
       </c>
@@ -1668,17 +1698,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
@@ -1686,7 +1716,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>31</v>
       </c>
@@ -1694,22 +1724,22 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>32</v>
       </c>
@@ -1717,7 +1747,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>33</v>
       </c>
@@ -1725,7 +1755,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>34</v>
       </c>
@@ -1733,17 +1763,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>35</v>
       </c>
@@ -1751,7 +1781,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>36</v>
       </c>
@@ -1759,17 +1789,17 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>37</v>
       </c>
@@ -1777,7 +1807,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>38</v>
       </c>
@@ -1785,7 +1815,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>39</v>
       </c>
@@ -1793,7 +1823,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>40</v>
       </c>
@@ -1801,7 +1831,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>41</v>
       </c>
@@ -1809,7 +1839,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>42</v>
       </c>
@@ -1817,7 +1847,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>43</v>
       </c>
@@ -1825,19 +1855,25 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>110</v>
+      </c>
+      <c r="C65" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>